<commit_message>
chegando proximo ao final do projeto
</commit_message>
<xml_diff>
--- a/storage/Produtos.xlsx
+++ b/storage/Produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,35 +446,95 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>Link Produto</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Lojas Americanas</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Magazine Luiza</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Preço Original</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Preço Atual</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
@@ -490,33 +550,69 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>iPhone 11 Apple 64GB Preto</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>https://www.amazon.com.br/Iphone-Apple-Preto-64gb-Desbloqueado/dp/B07SS4C6Y4/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=350014AADZE8M&amp;dchild=1&amp;keywords=iphone+64gb&amp;qid=1622839790&amp;sprefix=iphone+64%2Caps%2C305&amp;sr=8-1</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>https://www.americanas.com.br/produto/1611315933?pfm_carac=iphone-11-64gb-preto-ios-4g-camera-12mp-apple&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>https://www.magazineluiza.com.br/iphone-11-apple-64gb-preto-61-12mp-ios/p/155610500/te/ip11/</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="T2" t="n">
         <v>5297</v>
       </c>
-      <c r="I2" t="n">
+      <c r="U2" t="n">
         <v>3659.99</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>
@@ -532,33 +628,69 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>Smart TV 50" 4K LG 50UN7310PSC, UHD, WiFi, Bluetooth, HDR, Inteligência Artificial ThinQ AI, Smart Magic, Google e Alexa</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>https://www.amazon.com.br/Smart-LG-3LM631C0SB-Conversor-Digital/dp/B07WJX6PHL/ref=sr_1_3?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=Smart+TV+50%22+4K+LG+50UN7310PSC%2C+UHD%2C+WiFi%2C+Bluetooth%2C+HDR%2C+Intelig%C3%AAncia+Artificial+ThinQ+AI%2C+Smart+Magic%2C+Google+e+Alexa&amp;qid=1622869052&amp;sr=8-3</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>https://www.americanas.com.br/produto/2983614096?pfm_carac=smart-tv-50-lg-50un7310-uhd-4k-wifi-bluetooth-hdr-inteligencia-artificial-thinq-ai&amp;pfm_index=1&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>https://www.magazineluiza.com.br/smart-tv-uhd-4k-led-50-lg-50un7310psc-wi-fi-bluetooth-inteligencia-artificial-3-hdmi-2-usb/p/225376700/et/elit/?origin=autocomplete&amp;p=Smart%20TV%20LED%20PRO%2050%20Ultra%20HD%204K%20LG&amp;ranking=1&amp;typeclick=3&amp;ac_pos=header</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="T3" t="n">
         <v>2900</v>
       </c>
-      <c r="I3" t="n">
+      <c r="U3" t="n">
         <v>1999</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>

</xml_diff>

<commit_message>
ainda ha alguns pontos para trabalhar mas base do projeto finalizada
</commit_message>
<xml_diff>
--- a/storage/Produtos.xlsx
+++ b/storage/Produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:AU3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,35 +506,160 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
           <t>Link Produto</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Lojas Americanas</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Magazine Luiza</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Preço Original</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Preço Atual</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
@@ -586,35 +711,110 @@
       <c r="O2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="inlineStr">
         <is>
           <t>iPhone 11 Apple 64GB Preto</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>https://www.amazon.com.br/Iphone-Apple-Preto-64gb-Desbloqueado/dp/B07SS4C6Y4/ref=sr_1_1?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=350014AADZE8M&amp;dchild=1&amp;keywords=iphone+64gb&amp;qid=1622839790&amp;sprefix=iphone+64%2Caps%2C305&amp;sr=8-1</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>https://www.americanas.com.br/produto/1611315933?pfm_carac=iphone-11-64gb-preto-ios-4g-camera-12mp-apple&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>https://www.magazineluiza.com.br/iphone-11-apple-64gb-preto-61-12mp-ios/p/155610500/te/ip11/</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="AS2" t="n">
         <v>5297</v>
       </c>
-      <c r="U2" t="n">
-        <v>3659.99</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Amazon</t>
+      <c r="AT2" t="n">
+        <v>3905.07</v>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>Magalu</t>
         </is>
       </c>
     </row>
@@ -664,33 +864,108 @@
       <c r="O3" t="n">
         <v>1</v>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO3" t="inlineStr">
         <is>
           <t>Smart TV 50" 4K LG 50UN7310PSC, UHD, WiFi, Bluetooth, HDR, Inteligência Artificial ThinQ AI, Smart Magic, Google e Alexa</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="AP3" t="inlineStr">
         <is>
           <t>https://www.amazon.com.br/Smart-LG-3LM631C0SB-Conversor-Digital/dp/B07WJX6PHL/ref=sr_1_3?__mk_pt_BR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=Smart+TV+50%22+4K+LG+50UN7310PSC%2C+UHD%2C+WiFi%2C+Bluetooth%2C+HDR%2C+Intelig%C3%AAncia+Artificial+ThinQ+AI%2C+Smart+Magic%2C+Google+e+Alexa&amp;qid=1622869052&amp;sr=8-3</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>https://www.americanas.com.br/produto/2983614096?pfm_carac=smart-tv-50-lg-50un7310-uhd-4k-wifi-bluetooth-hdr-inteligencia-artificial-thinq-ai&amp;pfm_index=1&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="AR3" t="inlineStr">
         <is>
           <t>https://www.magazineluiza.com.br/smart-tv-uhd-4k-led-50-lg-50un7310psc-wi-fi-bluetooth-inteligencia-artificial-3-hdmi-2-usb/p/225376700/et/elit/?origin=autocomplete&amp;p=Smart%20TV%20LED%20PRO%2050%20Ultra%20HD%204K%20LG&amp;ranking=1&amp;typeclick=3&amp;ac_pos=header</t>
         </is>
       </c>
-      <c r="T3" t="n">
+      <c r="AS3" t="n">
         <v>2900</v>
       </c>
-      <c r="U3" t="n">
+      <c r="AT3" t="n">
         <v>1999</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="AU3" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>

</xml_diff>